<commit_message>
time and date bugs
</commit_message>
<xml_diff>
--- a/demo_attendance.xlsx
+++ b/demo_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\leave-analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEBE2C2-8B2D-4703-859C-49CD2F63D450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49D9175-5BB9-404A-9482-36474AC1B8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,30 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-02</t>
-  </si>
-  <si>
     <t>10:05</t>
   </si>
   <si>
     <t>18:30</t>
   </si>
   <si>
-    <t>2025-01-03</t>
-  </si>
-  <si>
     <t>09:55</t>
   </si>
   <si>
     <t>18:40</t>
-  </si>
-  <si>
-    <t>2025-01-04</t>
   </si>
   <si>
     <t>Employee Name</t>
@@ -99,12 +90,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -413,7 +408,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,59 +421,63 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45659</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45660</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45661</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="4">
+        <v>0.77361111111111114</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
         <v>45662</v>
       </c>
     </row>

</xml_diff>